<commit_message>
added clutter change functions
</commit_message>
<xml_diff>
--- a/blocks_final.xlsx
+++ b/blocks_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\repos\driving_sim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0F466B-C1DC-45CC-ADE1-BB65D5153267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B18D7FA7-DEDC-41E0-8654-8DC6C631B9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1428" yWindow="1428" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>training_lexical</t>
   </si>
   <si>
-    <t>training_driving_lexical</t>
-  </si>
-  <si>
     <t>task_name</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>full_task_eurostile</t>
+  </si>
+  <si>
+    <t>full_task_training</t>
   </si>
 </sst>
 </file>
@@ -441,7 +441,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -455,36 +455,36 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
       <c r="J1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -502,10 +502,10 @@
         <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2">
         <v>1.77</v>
@@ -516,10 +516,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -534,10 +534,10 @@
         <v>40</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I3">
         <v>1.77</v>
@@ -548,10 +548,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -566,10 +566,10 @@
         <v>40</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I4">
         <v>1.77</v>
@@ -580,10 +580,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
         <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -598,24 +598,24 @@
         <v>40</v>
       </c>
       <c r="G5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I5">
         <v>1.77</v>
       </c>
       <c r="J5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C6">
         <v>15</v>
@@ -630,10 +630,10 @@
         <v>4</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I6">
         <v>1.77</v>
@@ -644,10 +644,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>15</v>
@@ -662,10 +662,10 @@
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I7">
         <v>1.77</v>
@@ -676,10 +676,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>15</v>
@@ -694,10 +694,10 @@
         <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I8">
         <v>1.77</v>
@@ -708,10 +708,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9">
         <v>15</v>
@@ -726,16 +726,16 @@
         <v>6</v>
       </c>
       <c r="G9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I9">
         <v>1.77</v>
       </c>
       <c r="J9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
eurostile added for final clutter exp, final exp modified to accommodate changes in no clutter
</commit_message>
<xml_diff>
--- a/blocks_final.xlsx
+++ b/blocks_final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\repos\driving_sim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA84F425-FC18-4D4E-B14E-8B08ADBAA199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4556D5-9E6D-4ADD-BDDF-05E96A662D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1428" yWindow="1428" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>current_font</t>
   </si>
@@ -114,13 +114,25 @@
     <t>lexical_wo_driving_eurostile</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>full_task_eurostile</t>
   </si>
   <si>
     <t>full_task_training</t>
+  </si>
+  <si>
+    <t>maskEnabled</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
@@ -438,19 +450,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.88671875" customWidth="1"/>
+    <col min="1" max="1" width="33.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -481,8 +493,23 @@
       <c r="J1" t="s">
         <v>23</v>
       </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -496,10 +523,10 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
@@ -513,8 +540,23 @@
       <c r="J2">
         <v>2.0699999999999998</v>
       </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>20</v>
+      </c>
+      <c r="O2">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -528,10 +570,10 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
@@ -545,8 +587,23 @@
       <c r="J3">
         <v>1.9824999999999999</v>
       </c>
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>30</v>
+      </c>
+      <c r="O3">
+        <v>30</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -560,10 +617,10 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
@@ -577,8 +634,23 @@
       <c r="J4">
         <v>1.96</v>
       </c>
+      <c r="K4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>30</v>
+      </c>
+      <c r="O4">
+        <v>30</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -592,10 +664,10 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
@@ -606,28 +678,43 @@
       <c r="I5">
         <v>1.77</v>
       </c>
-      <c r="J5" t="s">
-        <v>26</v>
+      <c r="J5">
+        <v>2.14</v>
+      </c>
+      <c r="K5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>30</v>
+      </c>
+      <c r="O5">
+        <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
@@ -641,8 +728,23 @@
       <c r="J6">
         <v>2.0699999999999998</v>
       </c>
+      <c r="K6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6">
+        <v>5</v>
+      </c>
+      <c r="M6">
+        <v>10</v>
+      </c>
+      <c r="N6">
+        <v>8</v>
+      </c>
+      <c r="O6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -650,16 +752,16 @@
         <v>17</v>
       </c>
       <c r="C7">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G7" t="s">
         <v>9</v>
@@ -673,8 +775,23 @@
       <c r="J7">
         <v>1.9824999999999999</v>
       </c>
+      <c r="K7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7">
+        <v>5</v>
+      </c>
+      <c r="M7">
+        <v>10</v>
+      </c>
+      <c r="N7">
+        <v>12</v>
+      </c>
+      <c r="O7">
+        <v>12</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -682,16 +799,16 @@
         <v>18</v>
       </c>
       <c r="C8">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G8" t="s">
         <v>9</v>
@@ -705,25 +822,40 @@
       <c r="J8">
         <v>1.96</v>
       </c>
+      <c r="K8" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8">
+        <v>5</v>
+      </c>
+      <c r="M8">
+        <v>10</v>
+      </c>
+      <c r="N8">
+        <v>12</v>
+      </c>
+      <c r="O8">
+        <v>12</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -734,8 +866,23 @@
       <c r="I9">
         <v>1.77</v>
       </c>
-      <c r="J9" t="s">
-        <v>26</v>
+      <c r="J9">
+        <v>2.14</v>
+      </c>
+      <c r="K9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L9">
+        <v>5</v>
+      </c>
+      <c r="M9">
+        <v>10</v>
+      </c>
+      <c r="N9">
+        <v>12</v>
+      </c>
+      <c r="O9">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reverted trial counts to normal
</commit_message>
<xml_diff>
--- a/blocks_final.xlsx
+++ b/blocks_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4556D5-9E6D-4ADD-BDDF-05E96A662D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B73FAA-1E08-466E-A31D-2DEF9F056033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
   <si>
     <t>current_font</t>
   </si>
@@ -121,18 +121,6 @@
   </si>
   <si>
     <t>maskEnabled</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
   </si>
 </sst>
 </file>
@@ -450,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,7 +450,7 @@
     <col min="2" max="2" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -496,20 +484,8 @@
       <c r="K1" t="s">
         <v>28</v>
       </c>
-      <c r="L1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -523,10 +499,10 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
@@ -543,20 +519,8 @@
       <c r="K2" t="s">
         <v>9</v>
       </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>20</v>
-      </c>
-      <c r="O2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -570,10 +534,10 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
@@ -590,20 +554,8 @@
       <c r="K3" t="s">
         <v>9</v>
       </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3">
-        <v>30</v>
-      </c>
-      <c r="O3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -617,10 +569,10 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
@@ -637,20 +589,8 @@
       <c r="K4" t="s">
         <v>9</v>
       </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4">
-        <v>30</v>
-      </c>
-      <c r="O4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -664,10 +604,10 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
@@ -684,20 +624,8 @@
       <c r="K5" t="s">
         <v>9</v>
       </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <v>30</v>
-      </c>
-      <c r="O5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -705,16 +633,16 @@
         <v>27</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
@@ -731,20 +659,8 @@
       <c r="K6" t="s">
         <v>8</v>
       </c>
-      <c r="L6">
-        <v>5</v>
-      </c>
-      <c r="M6">
-        <v>10</v>
-      </c>
-      <c r="N6">
-        <v>8</v>
-      </c>
-      <c r="O6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -752,16 +668,16 @@
         <v>17</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
         <v>9</v>
@@ -778,20 +694,8 @@
       <c r="K7" t="s">
         <v>8</v>
       </c>
-      <c r="L7">
-        <v>5</v>
-      </c>
-      <c r="M7">
-        <v>10</v>
-      </c>
-      <c r="N7">
-        <v>12</v>
-      </c>
-      <c r="O7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -799,16 +703,16 @@
         <v>18</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s">
         <v>9</v>
@@ -825,20 +729,8 @@
       <c r="K8" t="s">
         <v>8</v>
       </c>
-      <c r="L8">
-        <v>5</v>
-      </c>
-      <c r="M8">
-        <v>10</v>
-      </c>
-      <c r="N8">
-        <v>12</v>
-      </c>
-      <c r="O8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -846,16 +738,16 @@
         <v>26</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -871,18 +763,6 @@
       </c>
       <c r="K9" t="s">
         <v>8</v>
-      </c>
-      <c r="L9">
-        <v>5</v>
-      </c>
-      <c r="M9">
-        <v>10</v>
-      </c>
-      <c r="N9">
-        <v>12</v>
-      </c>
-      <c r="O9">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added clutter counterbalance sheet, clutter change feature
</commit_message>
<xml_diff>
--- a/blocks_final.xlsx
+++ b/blocks_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B73FAA-1E08-466E-A31D-2DEF9F056033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0630EE0A-8DB9-4F8A-A43D-E7A8C19E3BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="855" windowWidth="25875" windowHeight="14175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
   <si>
     <t>current_font</t>
   </si>
@@ -121,6 +121,21 @@
   </si>
   <si>
     <t>maskEnabled</t>
+  </si>
+  <si>
+    <t>clutterChangeEnabled</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
@@ -438,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,7 +465,7 @@
     <col min="2" max="2" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,8 +499,23 @@
       <c r="K1" t="s">
         <v>28</v>
       </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -499,10 +529,10 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
@@ -519,8 +549,23 @@
       <c r="K2" t="s">
         <v>9</v>
       </c>
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>20</v>
+      </c>
+      <c r="P2">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -534,10 +579,10 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
@@ -554,8 +599,23 @@
       <c r="K3" t="s">
         <v>9</v>
       </c>
+      <c r="L3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>30</v>
+      </c>
+      <c r="P3">
+        <v>30</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -569,10 +629,10 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
@@ -589,8 +649,23 @@
       <c r="K4" t="s">
         <v>9</v>
       </c>
+      <c r="L4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>30</v>
+      </c>
+      <c r="P4">
+        <v>30</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -604,10 +679,10 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
@@ -624,8 +699,23 @@
       <c r="K5" t="s">
         <v>9</v>
       </c>
+      <c r="L5" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>30</v>
+      </c>
+      <c r="P5">
+        <v>30</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -633,16 +723,16 @@
         <v>27</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F6">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
@@ -659,8 +749,23 @@
       <c r="K6" t="s">
         <v>8</v>
       </c>
+      <c r="L6" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+      <c r="N6">
+        <v>10</v>
+      </c>
+      <c r="O6">
+        <v>20</v>
+      </c>
+      <c r="P6">
+        <v>20</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -668,10 +773,10 @@
         <v>17</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>12</v>
@@ -694,8 +799,23 @@
       <c r="K7" t="s">
         <v>8</v>
       </c>
+      <c r="L7" t="b">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
+      <c r="N7">
+        <v>10</v>
+      </c>
+      <c r="O7">
+        <v>12</v>
+      </c>
+      <c r="P7">
+        <v>12</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -703,10 +823,10 @@
         <v>18</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>12</v>
@@ -729,8 +849,23 @@
       <c r="K8" t="s">
         <v>8</v>
       </c>
+      <c r="L8" t="b">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>5</v>
+      </c>
+      <c r="N8">
+        <v>10</v>
+      </c>
+      <c r="O8">
+        <v>12</v>
+      </c>
+      <c r="P8">
+        <v>12</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -738,10 +873,10 @@
         <v>26</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>12</v>
@@ -763,6 +898,21 @@
       </c>
       <c r="K9" t="s">
         <v>8</v>
+      </c>
+      <c r="L9" t="b">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>5</v>
+      </c>
+      <c r="N9">
+        <v>10</v>
+      </c>
+      <c r="O9">
+        <v>12</v>
+      </c>
+      <c r="P9">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reverted blocks_final file to default
</commit_message>
<xml_diff>
--- a/blocks_final.xlsx
+++ b/blocks_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B253C2-6758-4F38-9F1E-BBD11317E5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47AE5A7-56A9-41AB-A0FC-9150B2583302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="345" yWindow="855" windowWidth="25875" windowHeight="14175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -444,7 +444,7 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,10 +505,10 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
@@ -555,10 +555,10 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
@@ -605,10 +605,10 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
@@ -655,10 +655,10 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
@@ -699,16 +699,16 @@
         <v>27</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
@@ -749,16 +749,16 @@
         <v>17</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
         <v>9</v>
@@ -799,16 +799,16 @@
         <v>18</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s">
         <v>9</v>
@@ -849,16 +849,16 @@
         <v>26</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
improved logic on clutter change, fixed crash bugs
</commit_message>
<xml_diff>
--- a/blocks_final.xlsx
+++ b/blocks_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47AE5A7-56A9-41AB-A0FC-9150B2583302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B06A61-32E8-4325-B287-02AE7DDCE56A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="345" yWindow="855" windowWidth="25875" windowHeight="14175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -441,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +453,7 @@
     <col min="2" max="2" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -491,7 +491,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -528,20 +528,8 @@
       <c r="L2" t="b">
         <v>0</v>
       </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>20</v>
-      </c>
-      <c r="P2">
-        <v>20</v>
-      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -578,20 +566,8 @@
       <c r="L3" t="b">
         <v>0</v>
       </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
-        <v>30</v>
-      </c>
-      <c r="P3">
-        <v>30</v>
-      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -628,20 +604,8 @@
       <c r="L4" t="b">
         <v>0</v>
       </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4">
-        <v>30</v>
-      </c>
-      <c r="P4">
-        <v>30</v>
-      </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -678,20 +642,8 @@
       <c r="L5" t="b">
         <v>0</v>
       </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="O5">
-        <v>30</v>
-      </c>
-      <c r="P5">
-        <v>30</v>
-      </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -728,20 +680,8 @@
       <c r="L6" t="b">
         <v>1</v>
       </c>
-      <c r="M6">
-        <v>5</v>
-      </c>
-      <c r="N6">
-        <v>10</v>
-      </c>
-      <c r="O6">
-        <v>20</v>
-      </c>
-      <c r="P6">
-        <v>20</v>
-      </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -778,20 +718,8 @@
       <c r="L7" t="b">
         <v>1</v>
       </c>
-      <c r="M7">
-        <v>5</v>
-      </c>
-      <c r="N7">
-        <v>10</v>
-      </c>
-      <c r="O7">
-        <v>12</v>
-      </c>
-      <c r="P7">
-        <v>12</v>
-      </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -828,20 +756,8 @@
       <c r="L8" t="b">
         <v>1</v>
       </c>
-      <c r="M8">
-        <v>5</v>
-      </c>
-      <c r="N8">
-        <v>10</v>
-      </c>
-      <c r="O8">
-        <v>12</v>
-      </c>
-      <c r="P8">
-        <v>12</v>
-      </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -877,18 +793,6 @@
       </c>
       <c r="L9" t="b">
         <v>1</v>
-      </c>
-      <c r="M9">
-        <v>5</v>
-      </c>
-      <c r="N9">
-        <v>10</v>
-      </c>
-      <c r="O9">
-        <v>12</v>
-      </c>
-      <c r="P9">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test version of driving+lexical w new icons
</commit_message>
<xml_diff>
--- a/blocks_final.xlsx
+++ b/blocks_final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B06A61-32E8-4325-B287-02AE7DDCE56A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978E3B5B-46D2-4C10-A558-A85DA36DDF64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="855" windowWidth="25875" windowHeight="14175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -443,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added an additional training block -full_task_wo_driving_training-
</commit_message>
<xml_diff>
--- a/blocks_final.xlsx
+++ b/blocks_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978E3B5B-46D2-4C10-A558-A85DA36DDF64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE295DB0-4084-4A92-B4BF-7792F0671FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
   <si>
     <t>current_font</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>clutterChangeEnabled</t>
+  </si>
+  <si>
+    <t>full_task_wo_driving_training</t>
   </si>
 </sst>
 </file>
@@ -441,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,7 +651,7 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -657,10 +660,10 @@
         <v>10</v>
       </c>
       <c r="E6">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F6">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
@@ -683,10 +686,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -695,22 +698,22 @@
         <v>10</v>
       </c>
       <c r="E7">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F7">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G7" t="s">
         <v>9</v>
       </c>
       <c r="H7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="I7">
         <v>1.77</v>
       </c>
       <c r="J7">
-        <v>1.9824999999999999</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="K7" t="s">
         <v>8</v>
@@ -721,10 +724,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -748,7 +751,7 @@
         <v>1.77</v>
       </c>
       <c r="J8">
-        <v>1.96</v>
+        <v>1.9824999999999999</v>
       </c>
       <c r="K8" t="s">
         <v>8</v>
@@ -759,10 +762,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -786,12 +789,50 @@
         <v>1.77</v>
       </c>
       <c r="J9">
-        <v>2.14</v>
+        <v>1.96</v>
       </c>
       <c r="K9" t="s">
         <v>8</v>
       </c>
       <c r="L9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>12</v>
+      </c>
+      <c r="F10">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10">
+        <v>1.77</v>
+      </c>
+      <c r="J10">
+        <v>2.14</v>
+      </c>
+      <c r="K10" t="s">
+        <v>8</v>
+      </c>
+      <c r="L10" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new instructions to new training blocks and to full clutter task
</commit_message>
<xml_diff>
--- a/blocks_final.xlsx
+++ b/blocks_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE295DB0-4084-4A92-B4BF-7792F0671FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B380E4C8-B568-4478-8BB1-A7B2C526C175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t>current_font</t>
   </si>
@@ -78,9 +78,6 @@
     <t>./instructions_pilot/lexical_task.png</t>
   </si>
   <si>
-    <t>./instructions_pilot/driving_lexical_training.png</t>
-  </si>
-  <si>
     <t>instruction_image_file</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>full_task_neuefrutigerworld</t>
   </si>
   <si>
-    <t>./instructions_pilot/full_task.png</t>
-  </si>
-  <si>
     <t>Georgia</t>
   </si>
   <si>
@@ -127,6 +121,15 @@
   </si>
   <si>
     <t>full_task_wo_driving_training</t>
+  </si>
+  <si>
+    <t>./instructions_pilot/full_task_clutter.png</t>
+  </si>
+  <si>
+    <t>./instructions_pilot/clutterlex_driving_training.png</t>
+  </si>
+  <si>
+    <t>./instructions_pilot/clutterlex_training.png</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,24 +482,24 @@
         <v>7</v>
       </c>
       <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
-        <v>16</v>
-      </c>
       <c r="J1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -534,7 +537,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -572,7 +575,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -610,10 +613,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -648,10 +651,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -669,7 +672,7 @@
         <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="I6">
         <v>1.77</v>
@@ -686,10 +689,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -707,7 +710,7 @@
         <v>9</v>
       </c>
       <c r="H7" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="I7">
         <v>1.77</v>
@@ -724,10 +727,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -745,7 +748,7 @@
         <v>9</v>
       </c>
       <c r="H8" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="I8">
         <v>1.77</v>
@@ -762,10 +765,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -783,7 +786,7 @@
         <v>9</v>
       </c>
       <c r="H9" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="I9">
         <v>1.77</v>
@@ -800,10 +803,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
         <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -821,7 +824,7 @@
         <v>9</v>
       </c>
       <c r="H10" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="I10">
         <v>1.77</v>

</xml_diff>

<commit_message>
fixed blocks_final spreadsheets that disabled clutter changes in the first training block
</commit_message>
<xml_diff>
--- a/blocks_final.xlsx
+++ b/blocks_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B380E4C8-B568-4478-8BB1-A7B2C526C175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46F3DC7-E34D-4CD3-8816-2545C2BDFF8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -450,7 +450,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fixed instruction image displays for the new training blocks
</commit_message>
<xml_diff>
--- a/blocks_final.xlsx
+++ b/blocks_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46F3DC7-E34D-4CD3-8816-2545C2BDFF8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFA99FD-02B2-461B-ADB3-AF5C29BE1C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -450,13 +450,14 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.7109375" customWidth="1"/>
     <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="8" max="8" width="64.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -669,7 +670,7 @@
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H6" t="s">
         <v>31</v>

</xml_diff>